<commit_message>
excel files with cards and symbols uploaded reading excel file with main.py
</commit_message>
<xml_diff>
--- a/Cards_Symbols.xlsx
+++ b/Cards_Symbols.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juergen/PycharmProjects/pythonDobble/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA819F07-4EDA-1243-93EE-88A00BAB9376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10BC8FE-E050-3742-A706-5D285A8BF351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="32160" xr2:uid="{DE9A87B5-78B3-B140-BFD3-5DD166B7043B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{DE9A87B5-78B3-B140-BFD3-5DD166B7043B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F0EBE-C4C2-B04A-BA63-2DE71C1DD129}">
   <dimension ref="A1:BF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="BH1" sqref="BH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>